<commit_message>
Se modifico el documeto de distribucion de trabajo
</commit_message>
<xml_diff>
--- a/Documentacion/Distribución de Trabajo.xlsx
+++ b/Documentacion/Distribución de Trabajo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC-10\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC-10\Documents\Proyecto\P.F\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E2DB90-6E92-4C04-80C9-B2ECB6549395}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077BE474-6EB2-4593-AE33-86CA2C4DB329}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" activeTab="1" xr2:uid="{AB28C158-560D-4BBB-BC35-7D89BF765275}"/>
   </bookViews>
@@ -660,54 +660,6 @@
     <t>Módulo 1 : Gestión de Compras
 Módulo 2:  Mantenimiento a Instalaciones
 Módulo 3:  Gestión de Inventarios  y Suministros</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Nombre: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">VAHUYA
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Integrantes: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Flores Valencia Jesus - 210336
-González Salazar Yair - 210256
-Sanchez Gonzalez Hugo - 200187</t>
-    </r>
   </si>
   <si>
     <t>Módulo 1 : Gestión de Miembros
@@ -2044,12 +1996,145 @@
   <si>
     <t>1.- Registro de Membresias</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Nombre: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">VAHUYA
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Integrantes: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Flores Valencia Jesus - 210336
+González Salazar Yair - 210256
+Sanchez Gonzalez Hugo - 200187
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">EQUIPO
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sanchez Gonzalez Hugo - 200187(Lider del proyecto)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+RESPONSABLE DEL FRONT Y BACK
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Sanchez Gonzalez Hugo - 200187(Lider del proyecto)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">RESPONSABLE DE LA DOCUMENTACION
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">González Salazar Yair - 210256
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">RESPONSABLE DE LA BASE DE DATOS
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Flores Valencia Jesus - 210336</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2104,6 +2189,14 @@
       <color rgb="FF000000"/>
       <name val="Docs-Calibri"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2138,7 +2231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2163,6 +2256,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2670,10 +2766,10 @@
         <v>12</v>
       </c>
       <c r="I4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="307.5" customHeight="1">
@@ -2684,19 +2780,19 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J5" s="2"/>
     </row>
@@ -2705,22 +2801,22 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J6" s="2"/>
     </row>
@@ -2735,16 +2831,16 @@
         <v>18</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J7" s="2"/>
     </row>
@@ -2759,16 +2855,16 @@
         <v>17</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J8" s="2"/>
     </row>
@@ -2784,7 +2880,7 @@
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -2806,13 +2902,13 @@
         <v>15</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J10" s="2"/>
     </row>
@@ -2830,7 +2926,7 @@
         <v>16</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -2849,10 +2945,10 @@
         <v>20</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -2865,22 +2961,22 @@
         <v>9</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J13" s="2"/>
     </row>
@@ -2934,8 +3030,8 @@
   <dimension ref="A2:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J8" sqref="J8"/>
+      <pane xSplit="2" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -2985,13 +3081,13 @@
         <v>12</v>
       </c>
       <c r="I4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="K4" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="44.25">
@@ -3006,13 +3102,13 @@
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -3031,18 +3127,18 @@
         <v>37</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="1"/>
       <c r="N6" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="257.25">
@@ -3059,20 +3155,20 @@
         <v>39</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="N7" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="281.25" customHeight="1">
@@ -3083,32 +3179,32 @@
         <v>27</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="E8" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="H8" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J8" s="8" t="s">
         <v>97</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>98</v>
       </c>
       <c r="K8" s="2"/>
       <c r="N8" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="279.75" customHeight="1">
@@ -3124,14 +3220,14 @@
       <c r="D9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>49</v>
+      <c r="E9" s="9" t="s">
+        <v>48</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -3150,16 +3246,16 @@
         <v>34</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K10" s="2"/>
     </row>
@@ -3171,19 +3267,19 @@
         <v>30</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -3202,13 +3298,13 @@
         <v>41</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>

</xml_diff>